<commit_message>
updated the excel with SLS A3 info
</commit_message>
<xml_diff>
--- a/Screen/Reporting Framework Screen info.xlsx
+++ b/Screen/Reporting Framework Screen info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aciesconsulting-my.sharepoint.com/personal/arushigupta_acies_holdings/Documents/Desktop/Arushi's handover/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeveshArya\Desktop\08-01-2025\Reporting-Framework\Screen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{CE940B08-05CA-474A-AF0C-57336043ED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C05C864-838E-4D24-A740-91B2FEE9EEBE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5932AB-A055-499E-BC23-3FD86424BD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{BDEEF678-FF6F-4AC3-A6F7-FEFFD510C599}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BDEEF678-FF6F-4AC3-A6F7-FEFFD510C599}"/>
   </bookViews>
   <sheets>
     <sheet name="System Framework" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="214">
   <si>
     <t>Computation Model</t>
   </si>
@@ -720,6 +720,12 @@
   </si>
   <si>
     <t>irs_report_output</t>
+  </si>
+  <si>
+    <t>SLS A3- Report</t>
+  </si>
+  <si>
+    <t>SLS A3</t>
   </si>
 </sst>
 </file>
@@ -1269,18 +1275,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30085C-4FA7-4403-BD3A-E9A8A79729F8}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1303,7 +1311,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1323,7 +1331,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1363,7 +1371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -1401,6 +1409,26 @@
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1412,18 +1440,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED77EE50-F772-4992-9737-9129948EF183}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1993,16 +2021,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" customWidth="1"/>
-    <col min="6" max="6" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>175</v>
       </c>
@@ -2012,7 +2040,7 @@
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>52</v>
       </c>
@@ -2032,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2052,7 +2080,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <f>A3+1</f>
         <v>2</v>
@@ -2073,7 +2101,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <f t="shared" ref="A5:A31" si="0">A4+1</f>
         <v>3</v>
@@ -2094,7 +2122,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2115,7 +2143,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2136,7 +2164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2157,7 +2185,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="93" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2178,7 +2206,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2199,7 +2227,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2220,7 +2248,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2241,7 +2269,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2262,7 +2290,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2283,7 +2311,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2304,7 +2332,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2325,7 +2353,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="93" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2346,7 +2374,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="93" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2367,7 +2395,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="93" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2388,7 +2416,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2409,7 +2437,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2430,7 +2458,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2451,7 +2479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="93" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2472,7 +2500,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2491,7 +2519,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2512,7 +2540,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2533,7 +2561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2554,7 +2582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2575,7 +2603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2596,7 +2624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2617,7 +2645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2654,12 +2682,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="88.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="88.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2696,7 +2724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A5" si="0">A3+1</f>
         <v>3</v>
@@ -2708,7 +2736,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2733,13 +2761,13 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>52</v>
       </c>
@@ -2747,7 +2775,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -2755,13 +2783,13 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="22"/>
       <c r="B3" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -2769,25 +2797,25 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="23"/>
       <c r="B6" s="16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" s="15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <v>3</v>
       </c>
@@ -2795,19 +2823,19 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="16" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="15" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <v>4</v>
       </c>
@@ -2815,13 +2843,13 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="15" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <v>5</v>
       </c>
@@ -2829,19 +2857,19 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="16" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <v>6</v>
       </c>
@@ -2849,7 +2877,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="15" t="s">
         <v>179</v>

</xml_diff>